<commit_message>
Add error raises in function get_indice() for indice majore Add some tests for indice_majore and gipa
</commit_message>
<xml_diff>
--- a/openfisca_france/assets/grilles_fonction_publique/test_grid.xlsx
+++ b/openfisca_france/assets/grilles_fonction_publique/test_grid.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="36">
   <si>
     <t>IB</t>
   </si>
@@ -168,12 +168,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30:L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,119 +1624,705 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="A30" s="1">
+        <v>20130101</v>
+      </c>
+      <c r="B30" s="3">
+        <v>20140131</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>12</v>
+      </c>
+      <c r="J30" s="1">
+        <v>12</v>
+      </c>
+      <c r="K30" s="1">
+        <v>306</v>
+      </c>
+      <c r="L30" s="1">
+        <v>312</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1444.65</v>
+      </c>
       <c r="N30" s="1"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="A31" s="1">
+        <v>20120101</v>
+      </c>
+      <c r="B31" s="3">
+        <v>20130101</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>12</v>
+      </c>
+      <c r="J31" s="1">
+        <v>12</v>
+      </c>
+      <c r="K31" s="1">
+        <v>306</v>
+      </c>
+      <c r="L31" s="1">
+        <v>312</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1444.65</v>
+      </c>
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>20110101</v>
+      </c>
+      <c r="B32" s="3">
+        <v>20120101</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>12</v>
+      </c>
+      <c r="J32" s="1">
+        <v>12</v>
+      </c>
+      <c r="K32" s="1">
+        <v>306</v>
+      </c>
+      <c r="L32" s="1">
+        <v>312</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>20100101</v>
+      </c>
+      <c r="B33" s="3">
+        <v>20110081</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>12</v>
+      </c>
+      <c r="J33" s="1">
+        <v>12</v>
+      </c>
+      <c r="K33" s="1">
+        <v>306</v>
+      </c>
+      <c r="L33" s="1">
+        <v>312</v>
+      </c>
+      <c r="M33" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>20090101</v>
+      </c>
+      <c r="B34" s="3">
+        <v>20100066</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1">
+        <v>12</v>
+      </c>
+      <c r="J34" s="1">
+        <v>12</v>
+      </c>
+      <c r="K34" s="1">
+        <v>306</v>
+      </c>
+      <c r="L34" s="1">
+        <v>312</v>
+      </c>
+      <c r="M34" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>20080101</v>
+      </c>
+      <c r="B35" s="3">
+        <v>20090051</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>12</v>
+      </c>
+      <c r="J35" s="1">
+        <v>12</v>
+      </c>
+      <c r="K35" s="1">
+        <v>306</v>
+      </c>
+      <c r="L35" s="1">
+        <v>312</v>
+      </c>
+      <c r="M35" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>20070101</v>
+      </c>
+      <c r="B36" s="3">
+        <v>20080036</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1">
+        <v>12</v>
+      </c>
+      <c r="J36" s="1">
+        <v>12</v>
+      </c>
+      <c r="K36" s="1">
+        <v>306</v>
+      </c>
+      <c r="L36" s="1">
+        <v>312</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>20060101</v>
+      </c>
+      <c r="B37" s="3">
+        <v>20070021</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <v>12</v>
+      </c>
+      <c r="J37" s="1">
+        <v>12</v>
+      </c>
+      <c r="K37" s="1">
+        <v>306</v>
+      </c>
+      <c r="L37" s="1">
+        <v>312</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>20050101</v>
+      </c>
+      <c r="B38" s="3">
+        <v>20060006</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1">
+        <v>12</v>
+      </c>
+      <c r="J38" s="1">
+        <v>12</v>
+      </c>
+      <c r="K38" s="1">
+        <v>306</v>
+      </c>
+      <c r="L38" s="1">
+        <v>312</v>
+      </c>
+      <c r="M38" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>20040101</v>
+      </c>
+      <c r="B39" s="3">
+        <v>20049991</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1">
+        <v>12</v>
+      </c>
+      <c r="J39" s="1">
+        <v>12</v>
+      </c>
+      <c r="K39" s="1">
+        <v>306</v>
+      </c>
+      <c r="L39" s="1">
+        <v>312</v>
+      </c>
+      <c r="M39" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>20030101</v>
+      </c>
+      <c r="B40" s="3">
+        <v>20039976</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>12</v>
+      </c>
+      <c r="J40" s="1">
+        <v>12</v>
+      </c>
+      <c r="K40" s="1">
+        <v>306</v>
+      </c>
+      <c r="L40" s="1">
+        <v>312</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>20020101</v>
+      </c>
+      <c r="B41" s="3">
+        <v>20029961</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>12</v>
+      </c>
+      <c r="J41" s="1">
+        <v>12</v>
+      </c>
+      <c r="K41" s="1">
+        <v>306</v>
+      </c>
+      <c r="L41" s="1">
+        <v>312</v>
+      </c>
+      <c r="M41" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>20010101</v>
+      </c>
+      <c r="B42" s="3">
+        <v>20019946</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="1">
+        <v>3</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>12</v>
+      </c>
+      <c r="J42" s="1">
+        <v>12</v>
+      </c>
+      <c r="K42" s="1">
+        <v>306</v>
+      </c>
+      <c r="L42" s="1">
+        <v>312</v>
+      </c>
+      <c r="M42" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>20000101</v>
+      </c>
+      <c r="B43" s="3">
+        <v>20009931</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G43" s="1">
+        <v>3</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>12</v>
+      </c>
+      <c r="J43" s="1">
+        <v>12</v>
+      </c>
+      <c r="K43" s="1">
+        <v>306</v>
+      </c>
+      <c r="L43" s="1">
+        <v>312</v>
+      </c>
+      <c r="M43" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>19990101</v>
+      </c>
+      <c r="B44" s="3">
+        <v>19999916</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="1">
+        <v>3</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1">
+        <v>12</v>
+      </c>
+      <c r="J44" s="1">
+        <v>12</v>
+      </c>
+      <c r="K44" s="1">
+        <v>306</v>
+      </c>
+      <c r="L44" s="1">
+        <v>312</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>19980101</v>
+      </c>
+      <c r="B45" s="3">
+        <v>19989901</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="1">
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1">
+        <v>12</v>
+      </c>
+      <c r="J45" s="1">
+        <v>12</v>
+      </c>
+      <c r="K45" s="1">
+        <v>306</v>
+      </c>
+      <c r="L45" s="1">
+        <v>312</v>
+      </c>
+      <c r="M45" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>19980101</v>
+      </c>
+      <c r="B46" s="3">
+        <v>19989901</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="1">
+        <v>3</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>12</v>
+      </c>
+      <c r="J46" s="1">
+        <v>12</v>
+      </c>
+      <c r="K46" s="1">
+        <v>306</v>
+      </c>
+      <c r="L46" s="1">
+        <v>312</v>
+      </c>
+      <c r="M46" s="1">
+        <v>1444.65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1742,7 +2331,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>

</xml_diff>

<commit_message>
Remove print Fix function gipa and gipa .yaml tests Add tib temps partiel and .yaml test
</commit_message>
<xml_diff>
--- a/openfisca_france/assets/grilles_fonction_publique/test_grid.xlsx
+++ b/openfisca_france/assets/grilles_fonction_publique/test_grid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="12915" windowHeight="4425"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="12915" windowHeight="4365"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -120,10 +120,10 @@
     <t>redacteur principal</t>
   </si>
   <si>
-    <t>redaceur chef</t>
-  </si>
-  <si>
     <t>date_effet_debut</t>
+  </si>
+  <si>
+    <t>redacteur chef</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30:L46"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +501,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>32</v>
@@ -1367,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G23" s="1">
         <v>3</v>
@@ -1403,7 +1403,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G24" s="1">
         <v>3</v>
@@ -1442,7 +1442,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G25" s="1">
         <v>3</v>
@@ -1481,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G26" s="1">
         <v>3</v>
@@ -1520,7 +1520,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G27" s="1">
         <v>3</v>
@@ -1559,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G28" s="1">
         <v>3</v>
@@ -1598,7 +1598,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G29" s="1">
         <v>3</v>
@@ -1640,7 +1640,7 @@
         <v>7</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G30" s="1">
         <v>1</v>
@@ -1682,7 +1682,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
@@ -1724,7 +1724,7 @@
         <v>7</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -1765,7 +1765,7 @@
         <v>7</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -1806,7 +1806,7 @@
         <v>7</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
@@ -1847,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G35" s="1">
         <v>1</v>
@@ -1888,7 +1888,7 @@
         <v>7</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -1929,7 +1929,7 @@
         <v>7</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G37" s="1">
         <v>2</v>
@@ -1970,7 +1970,7 @@
         <v>7</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G38" s="1">
         <v>2</v>
@@ -2011,7 +2011,7 @@
         <v>7</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G39" s="1">
         <v>2</v>
@@ -2052,7 +2052,7 @@
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G40" s="1">
         <v>2</v>
@@ -2093,7 +2093,7 @@
         <v>7</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G41" s="1">
         <v>2</v>
@@ -2134,7 +2134,7 @@
         <v>7</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G42" s="1">
         <v>3</v>
@@ -2175,7 +2175,7 @@
         <v>7</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G43" s="1">
         <v>3</v>
@@ -2216,7 +2216,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G44" s="1">
         <v>3</v>
@@ -2257,7 +2257,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G45" s="1">
         <v>3</v>
@@ -2298,7 +2298,7 @@
         <v>7</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G46" s="1">
         <v>3</v>

</xml_diff>